<commit_message>
ADD: tablas para importar el BOM y calcular costes de manufacturación
</commit_message>
<xml_diff>
--- a/docs/Unkeyboard_project_planning.xlsx
+++ b/docs/Unkeyboard_project_planning.xlsx
@@ -3,11 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Project schedule" sheetId="1" state="visible" r:id="rId4"/>
-    <sheet name="Priority list" sheetId="2" state="visible" r:id="rId5"/>
+    <sheet name="Project schedule" sheetId="1" state="visible" r:id="rId5"/>
+    <sheet name="Priority list" sheetId="2" state="visible" r:id="rId6"/>
+    <sheet name="Manufacturing" sheetId="3" state="visible" r:id="rId7"/>
+    <sheet name="BOM" sheetId="4" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Print_Titles" localSheetId="0">'Project schedule'!$4:$6</definedName>
@@ -812,7 +814,7 @@
     <xf fontId="5" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="6" fillId="3" borderId="3" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="12" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -1115,9 +1117,6 @@
     </xf>
     <xf fontId="0" fillId="15" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="15" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2818,12 +2817,12 @@
       </c>
       <c r="F12" s="59">
         <f ca="1">TODAY()</f>
-        <v>45190</v>
+        <v>45197</v>
       </c>
       <c r="G12" s="45"/>
       <c r="H12" s="46">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I12" s="53"/>
       <c r="J12" s="53"/>
@@ -4514,7 +4513,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="37" stopIfTrue="1" id="{00FC0098-00B7-45D5-B1A1-00050058005D}">
+          <x14:cfRule type="expression" priority="37" stopIfTrue="1" id="{0004007C-00C5-43AC-9962-00600092005A}">
             <xm:f>AND(task_end&gt;=I$5,task_start&lt;J$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4535,7 +4534,7 @@
           <xm:sqref>I29:BL33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="36" id="{00C000AE-00D9-477E-868B-00EC007B00FC}">
+          <x14:cfRule type="expression" priority="36" id="{0018001D-001F-4BBF-AD57-001B003A0030}">
             <xm:f>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4556,7 +4555,7 @@
           <xm:sqref>I29:BL33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="23" id="{002F00F0-0056-46A9-881C-008200C5000A}">
+          <x14:cfRule type="dataBar" priority="23" id="{004500A9-0051-4359-8C95-00D500940017}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -4572,7 +4571,7 @@
           <xm:sqref>D7:D13 D15:D35 D14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" stopIfTrue="1" id="{002D00ED-00BE-4ECF-B5D9-005B00B6001A}">
+          <x14:cfRule type="expression" priority="7" stopIfTrue="1" id="{00AE00A2-002B-4B53-BE29-0075001200BF}">
             <xm:f>AND(task_end&gt;=I$5,task_start&lt;J$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4597,7 +4596,7 @@
           <xm:sqref>I9:BL15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{00A600E7-00FD-47A9-8679-006500F20016}">
+          <x14:cfRule type="expression" priority="6" id="{00F8006D-005B-42C8-B81F-00DF000300BD}">
             <xm:f>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4622,7 +4621,7 @@
           <xm:sqref>I9:BL15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" stopIfTrue="1" id="{00B700B7-0024-4FAD-8C48-007600D40078}">
+          <x14:cfRule type="expression" priority="5" stopIfTrue="1" id="{00BE006D-003A-4FA7-82BE-001D00880096}">
             <xm:f>AND(task_end&gt;=I$5,task_start&lt;J$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4647,7 +4646,7 @@
           <xm:sqref>I17:BL21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="4" id="{00A900C2-00E8-4B8F-83C2-00F7003900E9}">
+          <x14:cfRule type="expression" priority="4" id="{0053006C-00BE-4894-A55B-0015004300CE}">
             <xm:f>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4661,7 +4660,7 @@
           <xm:sqref>I17:BL21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" stopIfTrue="1" id="{00F1009A-0002-43DB-BB33-0015001D009E}">
+          <x14:cfRule type="expression" priority="3" stopIfTrue="1" id="{00CA00D1-00F1-420D-BEB1-004E00E200D0}">
             <xm:f>AND(task_end&gt;=I$5,task_start&lt;J$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4686,7 +4685,7 @@
           <xm:sqref>I23:BL27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{00750044-00C4-4EFD-9BB2-00DC00FF00F5}">
+          <x14:cfRule type="expression" priority="2" id="{00A200B5-00A0-400C-93F3-003300B000F4}">
             <xm:f>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</xm:f>
             <x14:dxf>
               <fill>
@@ -4711,7 +4710,7 @@
           <xm:sqref>I23:BL27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{00C800FC-0023-4DDE-AC0B-006C00BA0098}">
+          <x14:cfRule type="expression" priority="1" id="{00DB008D-0064-400D-A387-00F700D20028}">
             <xm:f>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</xm:f>
             <x14:dxf>
               <border>
@@ -4735,7 +4734,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007A0094-001D-4EDC-BBFE-005B00F4005C}" type="whole" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="greaterThanOrEqual" prompt="Changing this number will scroll the Gantt Chart view." promptTitle="Display Week" showDropDown="0" showErrorMessage="0" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0030008F-006F-4E60-8B28-000300A200A7}" type="whole" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="greaterThanOrEqual" prompt="Changing this number will scroll the Gantt Chart view." promptTitle="Display Week" showDropDown="0" showErrorMessage="0" showInputMessage="1">
           <x14:formula1>
             <xm:f>1</xm:f>
           </x14:formula1>
@@ -4827,7 +4826,7 @@
       </c>
     </row>
     <row r="9" ht="28.5">
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="109" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="110">
@@ -4854,7 +4853,7 @@
       <c r="B12" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="112">
+      <c r="C12" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4862,7 +4861,7 @@
       <c r="B13" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="112">
+      <c r="C13" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4870,7 +4869,7 @@
       <c r="B14" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="112">
+      <c r="C14" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4878,7 +4877,7 @@
       <c r="B15" s="109" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="112">
+      <c r="C15" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4886,7 +4885,7 @@
       <c r="B16" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="112">
+      <c r="C16" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4894,7 +4893,7 @@
       <c r="B17" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="112">
+      <c r="C17" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4902,7 +4901,7 @@
       <c r="B18" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="112">
+      <c r="C18" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4910,7 +4909,7 @@
       <c r="B19" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="112">
+      <c r="C19" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4918,7 +4917,7 @@
       <c r="B20" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="112">
+      <c r="C20" s="111">
         <v>3</v>
       </c>
     </row>
@@ -4926,7 +4925,7 @@
       <c r="B21" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="112">
+      <c r="C21" s="111">
         <v>4</v>
       </c>
     </row>
@@ -4934,7 +4933,7 @@
       <c r="B22" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="112">
+      <c r="C22" s="111">
         <v>5</v>
       </c>
     </row>
@@ -4942,7 +4941,7 @@
       <c r="B23" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="112">
+      <c r="C23" s="111">
         <v>5</v>
       </c>
     </row>
@@ -4950,7 +4949,7 @@
       <c r="B24" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="112">
+      <c r="C24" s="111">
         <v>5</v>
       </c>
     </row>
@@ -4958,7 +4957,7 @@
       <c r="B25" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="112">
+      <c r="C25" s="111">
         <v>5</v>
       </c>
     </row>
@@ -4966,7 +4965,7 @@
       <c r="B26" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="112">
+      <c r="C26" s="111">
         <v>5</v>
       </c>
     </row>
@@ -4974,7 +4973,7 @@
       <c r="B27" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="112">
+      <c r="C27" s="111">
         <v>5</v>
       </c>
     </row>
@@ -5042,7 +5041,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="5" id="{00A10006-0082-4CAC-A52B-00E700AA003A}">
+          <x14:cfRule type="duplicateValues" priority="5" id="{00C30028-0025-48CF-A9FF-005400DE0051}">
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -5063,36 +5062,39 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5404,12 +5406,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5432,5 +5459,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>